<commit_message>
2024/07/24 Finish the last efset -30 plot and fix some bug
</commit_message>
<xml_diff>
--- a/data/internal resistance/21700E_IR.xlsx
+++ b/data/internal resistance/21700E_IR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shane\Desktop\Battery_lowtemperature\pythonProject\data\internal resistance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F994037-04A0-42E9-A5D8-2BB3B2C93B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3F6133-E7D2-4A69-BA2C-A7BBFCB0919C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="20" windowWidth="22540" windowHeight="14300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -380,7 +380,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -527,18 +527,54 @@
       <c r="A6">
         <v>-25</v>
       </c>
-      <c r="G6" t="e">
+      <c r="B6">
+        <v>9925</v>
+      </c>
+      <c r="C6">
+        <v>4.1036000000000001</v>
+      </c>
+      <c r="D6">
+        <v>3.5800999999999998</v>
+      </c>
+      <c r="E6">
+        <v>-1.07E-3</v>
+      </c>
+      <c r="F6">
+        <v>-3.9947499999999998</v>
+      </c>
+      <c r="G6">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.1310821097333788</v>
+      </c>
+      <c r="H6">
+        <v>69.900000000000006</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>-30</v>
       </c>
-      <c r="G7" t="e">
+      <c r="B7">
+        <v>10145</v>
+      </c>
+      <c r="C7">
+        <v>4.0776000000000003</v>
+      </c>
+      <c r="D7">
+        <v>3.4533499999999999</v>
+      </c>
+      <c r="E7">
+        <v>-1.06E-3</v>
+      </c>
+      <c r="F7">
+        <v>-3.9948000000000001</v>
+      </c>
+      <c r="G7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.15630712064380764</v>
+      </c>
+      <c r="H7">
+        <v>65.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>